<commit_message>
incluindo rotina que monta o "ensemble" por Ano, Cenário e Replicação, Considerando que as Variáveis informadas nem sempre serão as mesmas
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$S$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$H$26</definedName>
     <definedName name="Ano_Inicial">Configs!$D$2:$D$2</definedName>
     <definedName name="Anos_a_Serem_Simulados">Configs!$A$2</definedName>
     <definedName name="CategoriaSAT">Configs!$C$2:$C$2</definedName>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="75">
   <si>
     <t>Ano</t>
   </si>
@@ -247,10 +247,16 @@
     <t>Replicacoes</t>
   </si>
   <si>
-    <t>CenarioASimular</t>
-  </si>
-  <si>
     <t>Simular</t>
+  </si>
+  <si>
+    <t>Cenario</t>
+  </si>
+  <si>
+    <t>CenarioASIS</t>
+  </si>
+  <si>
+    <t>VariavelNova</t>
   </si>
 </sst>
 </file>
@@ -752,7 +758,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,27 +1161,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
@@ -1183,8 +1193,12 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
@@ -1192,8 +1206,12 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>43</v>
       </c>
@@ -1201,26 +1219,38 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B6" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>57</v>
       </c>
@@ -1228,8 +1258,12 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>58</v>
       </c>
@@ -1237,8 +1271,12 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>59</v>
       </c>
@@ -1246,8 +1284,12 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>60</v>
       </c>
@@ -1255,8 +1297,12 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>61</v>
       </c>
@@ -1264,8 +1310,12 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>62</v>
       </c>
@@ -1273,14 +1323,22 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B13" t="b">
         <f>TRUE</f>
         <v>1</v>
+      </c>
+      <c r="C13" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1291,11 +1349,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S17"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:S1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1305,14 +1362,10 @@
     <col min="4" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1335,43 +1388,10 @@
         <v>63</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1387,56 +1407,11 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1453,56 +1428,11 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1518,56 +1448,11 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1585,56 +1470,11 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S5" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1650,56 +1490,11 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I6" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1717,56 +1512,11 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I7" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S7" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1782,56 +1532,11 @@
       <c r="G8">
         <v>2</v>
       </c>
-      <c r="H8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I8" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S8" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1849,56 +1554,11 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I9" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1914,56 +1574,11 @@
       <c r="G10">
         <v>2</v>
       </c>
-      <c r="H10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J10" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S10" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1980,56 +1595,11 @@
       <c r="G11">
         <v>2</v>
       </c>
-      <c r="H11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -2045,56 +1615,11 @@
       <c r="G12">
         <v>2</v>
       </c>
-      <c r="H12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J12" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S12" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2112,56 +1637,11 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J13" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S13" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2177,56 +1657,11 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R14" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S14" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H14" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -2243,56 +1678,11 @@
       <c r="G15">
         <v>2</v>
       </c>
-      <c r="H15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R15" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S15" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H15" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -2308,56 +1698,11 @@
       <c r="G16">
         <v>2</v>
       </c>
-      <c r="H16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S16" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H16" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2375,62 +1720,303 @@
       <c r="G17">
         <v>2</v>
       </c>
-      <c r="H17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Q17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="R17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="S17" t="b">
-        <f>TRUE()</f>
+      <c r="H17" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="10">
+        <v>12</v>
+      </c>
+      <c r="D19" s="10">
+        <f>D18*1.1</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="10">
+        <f>C20+1</f>
+        <v>5</v>
+      </c>
+      <c r="D21" s="10">
+        <f>D20*1.1</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="G23">
         <v>1</v>
       </c>
+      <c r="H23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="10">
+        <v>12</v>
+      </c>
+      <c r="D28" s="10">
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="10">
+        <v>5</v>
+      </c>
+      <c r="D30" s="10">
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S17"/>
+  <autoFilter ref="A1:H26">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Iniciativa3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="I6 I7:J13" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
implementação da função obter_parametros(). Observar resultados com os parâmetros gerados no arquivo parametros_gerados.csv
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$H$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$H$33</definedName>
     <definedName name="Ano_Inicial">Configs!$D$2:$D$2</definedName>
     <definedName name="Anos_a_Serem_Simulados">Configs!$A$2</definedName>
     <definedName name="CategoriaSAT">Configs!$C$2:$C$2</definedName>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="74">
   <si>
     <t>Ano</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>CenarioASIS</t>
-  </si>
-  <si>
-    <t>VariavelNova</t>
   </si>
 </sst>
 </file>
@@ -1163,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,8 +1226,8 @@
         <v>55</v>
       </c>
       <c r="B5" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="C5" t="b">
         <f>FALSE</f>
@@ -1242,8 +1239,8 @@
         <v>56</v>
       </c>
       <c r="B6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="C6" t="b">
         <f>FALSE</f>
@@ -1349,10 +1346,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H21" sqref="A18:H21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1391,7 +1389,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1411,7 +1409,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1432,7 +1430,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1452,7 +1450,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1474,7 +1472,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1494,7 +1492,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1516,7 +1514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1536,7 +1534,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1558,7 +1556,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1578,7 +1576,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1599,7 +1597,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1619,7 +1617,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1641,7 +1639,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1661,7 +1659,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -1682,7 +1680,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1702,7 +1700,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1724,297 +1722,27 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="10">
-        <v>12</v>
-      </c>
-      <c r="D19" s="10">
-        <f>D18*1.1</f>
-        <v>3.3000000000000003</v>
-      </c>
-      <c r="G19">
-        <v>2</v>
-      </c>
-      <c r="H19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="H20" t="s">
-        <v>55</v>
-      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="10">
-        <f>C20+1</f>
-        <v>5</v>
-      </c>
-      <c r="D21" s="10">
-        <f>D20*1.1</f>
-        <v>3.3000000000000003</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23">
-        <v>8</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24">
-        <v>7</v>
-      </c>
-      <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="G24">
-        <v>2</v>
-      </c>
-      <c r="H24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25">
-        <v>7</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26">
-        <v>7</v>
-      </c>
-      <c r="D26">
-        <v>3</v>
-      </c>
-      <c r="G26">
-        <v>2</v>
-      </c>
-      <c r="H26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27">
-        <v>7</v>
-      </c>
-      <c r="D27">
-        <v>3</v>
-      </c>
-      <c r="G27">
-        <v>2</v>
-      </c>
-      <c r="H27" t="s">
-        <v>56</v>
-      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="10">
-        <v>12</v>
-      </c>
-      <c r="D28" s="10">
-        <v>3.3000000000000003</v>
-      </c>
-      <c r="G28">
-        <v>2</v>
-      </c>
-      <c r="H28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <v>3</v>
-      </c>
-      <c r="G29">
-        <v>2</v>
-      </c>
-      <c r="H29" t="s">
-        <v>56</v>
-      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="10">
-        <v>5</v>
-      </c>
-      <c r="D30" s="10">
-        <v>3.3000000000000003</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31">
-        <v>7</v>
-      </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
-      <c r="H31" t="s">
-        <v>56</v>
-      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H26">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Iniciativa3"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H33"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
calculo de despesas em absenteismo, primeiro app shiny com calculo de absenteeismo
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Dados_Projetados" sheetId="2" r:id="rId3"/>
     <sheet name="Cenarios" sheetId="9" r:id="rId4"/>
     <sheet name="Parametros" sheetId="4" r:id="rId5"/>
-    <sheet name="Custos_Iniciativas" sheetId="8" r:id="rId6"/>
+    <sheet name="Custos" sheetId="8" r:id="rId6"/>
     <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="73">
   <si>
     <t>Ano</t>
   </si>
@@ -232,15 +232,9 @@
     <t>TestarIniciativasEmConjunto?</t>
   </si>
   <si>
-    <t>Iniciativa</t>
-  </si>
-  <si>
     <t>Categoria</t>
   </si>
   <si>
-    <t>Custo</t>
-  </si>
-  <si>
     <t>Custo Total</t>
   </si>
   <si>
@@ -254,6 +248,9 @@
   </si>
   <si>
     <t>CenarioASIS</t>
+  </si>
+  <si>
+    <t>CustoTotal</t>
   </si>
 </sst>
 </file>
@@ -780,7 +777,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -1160,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,13 +1170,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1348,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="A18:H21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,7 +1383,7 @@
         <v>63</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1438,10 +1435,10 @@
         <v>19</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1E-3</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1457,13 +1454,11 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="10">
-        <f>C4+1</f>
-        <v>11</v>
-      </c>
-      <c r="D5" s="10">
-        <f>D4*1.1</f>
-        <v>3.3000000000000003</v>
+      <c r="C5">
+        <v>0.1</v>
+      </c>
+      <c r="D5">
+        <v>1E-3</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -1480,7 +1475,7 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1500,8 +1495,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="10">
-        <f>C6+1</f>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D7" s="10">
         <f>D6*1.1</f>
@@ -1522,10 +1516,10 @@
         <v>19</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>1E-3</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -1541,13 +1535,11 @@
       <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="10">
-        <f>C8+1</f>
-        <v>6</v>
-      </c>
-      <c r="D9" s="10">
-        <f>D8*1.1</f>
-        <v>3.3000000000000003</v>
+      <c r="C9">
+        <v>0.05</v>
+      </c>
+      <c r="D9">
+        <v>1E-3</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1605,10 +1597,10 @@
         <v>19</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>1E-3</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -1624,13 +1616,11 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="10">
-        <f>C12+1</f>
-        <v>5</v>
-      </c>
-      <c r="D13" s="10">
-        <f>D12*1.1</f>
-        <v>3.3000000000000003</v>
+      <c r="C13">
+        <v>0.05</v>
+      </c>
+      <c r="D13">
+        <v>1E-3</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1688,10 +1678,10 @@
         <v>19</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>1E-3</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -1707,13 +1697,11 @@
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="10">
-        <f>C16+1</f>
-        <v>5</v>
-      </c>
-      <c r="D17" s="10">
-        <f>D16*1.1</f>
-        <v>3.3000000000000003</v>
+      <c r="C17">
+        <v>0.05</v>
+      </c>
+      <c r="D17">
+        <v>1E-3</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -1750,29 +1738,32 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="12" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1780,13 +1771,13 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="13">
         <v>2017</v>
       </c>
       <c r="D2" s="4">
-        <v>50</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1794,13 +1785,13 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="13">
         <v>2018</v>
       </c>
       <c r="D3" s="4">
-        <v>20</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1808,13 +1799,13 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="13">
         <v>2019</v>
       </c>
       <c r="D4" s="4">
-        <v>20</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1822,13 +1813,13 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" s="13">
         <v>2020</v>
       </c>
       <c r="D5" s="4">
-        <v>20</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1836,13 +1827,13 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="13">
         <v>2021</v>
       </c>
       <c r="D6" s="4">
-        <v>20</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1850,14 +1841,14 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="13">
         <v>2017</v>
       </c>
       <c r="D7" s="4">
         <f>D2*2</f>
-        <v>100</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1865,14 +1856,14 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="13">
         <v>2018</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" ref="D8:D11" si="0">D3*2</f>
-        <v>40</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1880,14 +1871,14 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="13">
         <v>2019</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1895,14 +1886,14 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="13">
         <v>2020</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1910,14 +1901,154 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="13">
         <v>2021</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="13">
+        <v>2017</v>
+      </c>
+      <c r="D12" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="13">
+        <v>2018</v>
+      </c>
+      <c r="D13" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="13">
+        <v>2019</v>
+      </c>
+      <c r="D14" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="13">
+        <v>2020</v>
+      </c>
+      <c r="D15" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="13">
+        <v>2021</v>
+      </c>
+      <c r="D16" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="13">
+        <v>2017</v>
+      </c>
+      <c r="D17" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="13">
+        <v>2018</v>
+      </c>
+      <c r="D18" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="13">
+        <v>2019</v>
+      </c>
+      <c r="D19" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="13">
+        <v>2020</v>
+      </c>
+      <c r="D20" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="13">
+        <v>2021</v>
+      </c>
+      <c r="D21" s="4">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Implementando Distribuição Triangular; \n- Corrigindo Bug na Distribuição Uniforme.
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -12,8 +12,9 @@
     <sheet name="Dados_Projetados" sheetId="2" r:id="rId3"/>
     <sheet name="Cenarios" sheetId="9" r:id="rId4"/>
     <sheet name="Parametros" sheetId="4" r:id="rId5"/>
-    <sheet name="Custos" sheetId="8" r:id="rId6"/>
-    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId7"/>
+    <sheet name="Distribuições" sheetId="10" r:id="rId6"/>
+    <sheet name="Custos" sheetId="8" r:id="rId7"/>
+    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="85">
   <si>
     <t>Ano</t>
   </si>
@@ -91,9 +92,6 @@
     <t>Distribuicao</t>
   </si>
   <si>
-    <t>norm</t>
-  </si>
-  <si>
     <t>TaxaDeDesconto</t>
   </si>
   <si>
@@ -251,6 +249,45 @@
   </si>
   <si>
     <t>CustoTotal</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>triangular</t>
+  </si>
+  <si>
+    <t>Distribuição</t>
+  </si>
+  <si>
+    <t>Parametro 1</t>
+  </si>
+  <si>
+    <t>Parametro 2</t>
+  </si>
+  <si>
+    <t>Parametro 3</t>
+  </si>
+  <si>
+    <t>Parametro 4</t>
+  </si>
+  <si>
+    <t>uniforme</t>
+  </si>
+  <si>
+    <t>média</t>
+  </si>
+  <si>
+    <t>desvio padrão</t>
+  </si>
+  <si>
+    <t>mínimo</t>
+  </si>
+  <si>
+    <t>máximo</t>
+  </si>
+  <si>
+    <t>moda (valor mais provável)</t>
   </si>
 </sst>
 </file>
@@ -666,78 +703,78 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -777,7 +814,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -789,43 +826,43 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -855,10 +892,10 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
         <v>25</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -918,10 +955,10 @@
         <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1170,18 +1207,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="b">
         <f>TRUE</f>
@@ -1207,7 +1244,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="b">
         <f>TRUE</f>
@@ -1220,7 +1257,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="b">
         <f>FALSE</f>
@@ -1233,7 +1270,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" t="b">
         <f>FALSE</f>
@@ -1246,7 +1283,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="b">
         <f>FALSE</f>
@@ -1259,7 +1296,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" t="b">
         <f>FALSE</f>
@@ -1272,7 +1309,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" t="b">
         <f>FALSE</f>
@@ -1285,7 +1322,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="b">
         <f>FALSE</f>
@@ -1298,7 +1335,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="b">
         <f>FALSE</f>
@@ -1311,7 +1348,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" t="b">
         <f>FALSE</f>
@@ -1324,7 +1361,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" t="b">
         <f>TRUE</f>
@@ -1349,16 +1386,16 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" customWidth="1"/>
   </cols>
@@ -1383,18 +1420,18 @@
         <v>15</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1406,15 +1443,15 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C3" s="10">
         <v>20</v>
@@ -1427,15 +1464,15 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -1447,15 +1484,15 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C5">
         <v>0.1</v>
@@ -1467,15 +1504,15 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -1492,10 +1529,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C7" s="10">
         <v>20</v>
@@ -1513,10 +1550,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C8">
         <v>0.05</v>
@@ -1533,10 +1570,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C9">
         <v>0.05</v>
@@ -1553,164 +1590,186 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="C11" s="10">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D11" s="10">
-        <f>D10*1.1</f>
-        <v>3.3000000000000003</v>
+        <v>10</v>
       </c>
       <c r="G11">
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="C12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D12">
-        <v>1E-3</v>
+        <v>0.08</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E17" si="0">D12*1.2</f>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="C13">
         <v>0.05</v>
       </c>
       <c r="D13">
-        <v>1E-3</v>
+        <v>0.08</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
         <v>7</v>
       </c>
-      <c r="D14">
-        <v>3</v>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="C15" s="10">
+        <v>9</v>
+      </c>
+      <c r="D15" s="10">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
         <v>12</v>
-      </c>
-      <c r="D15" s="10">
-        <f>D14*1.1</f>
-        <v>3.3000000000000003</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="C16">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D16">
-        <v>1E-3</v>
+        <v>0.08</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="G16">
         <v>2</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="C17">
         <v>0.05</v>
       </c>
       <c r="D17">
-        <v>1E-3</v>
+        <v>0.08</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="G17">
         <v>2</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1740,6 +1799,80 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -1757,16 +1890,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1774,7 +1907,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="13">
         <v>2017</v>
@@ -1788,7 +1921,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="13">
         <v>2018</v>
@@ -1802,7 +1935,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="13">
         <v>2019</v>
@@ -1816,7 +1949,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="13">
         <v>2020</v>
@@ -1830,7 +1963,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="13">
         <v>2021</v>
@@ -1841,10 +1974,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="13">
         <v>2017</v>
@@ -1856,10 +1989,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="13">
         <v>2018</v>
@@ -1871,10 +2004,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="13">
         <v>2019</v>
@@ -1886,10 +2019,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="13">
         <v>2020</v>
@@ -1901,10 +2034,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="13">
         <v>2021</v>
@@ -1916,10 +2049,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="13">
         <v>2017</v>
@@ -1930,10 +2063,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="13">
         <v>2018</v>
@@ -1944,10 +2077,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="13">
         <v>2019</v>
@@ -1958,10 +2091,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="13">
         <v>2020</v>
@@ -1972,10 +2105,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="13">
         <v>2021</v>
@@ -1986,10 +2119,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="13">
         <v>2017</v>
@@ -2000,10 +2133,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="13">
         <v>2018</v>
@@ -2014,10 +2147,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="13">
         <v>2019</v>
@@ -2028,10 +2161,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="13">
         <v>2020</v>
@@ -2042,10 +2175,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="13">
         <v>2021</v>
@@ -2059,7 +2192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
#1 Criando Fluxo de Caixa Descontado
 - Agora as variáveis definidas no vetor variaveis_a_descontar são duplicadas e descontadas em novas variaveis.
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +882,7 @@
         <v>123412321</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
#2 Implementada a Função calcular_cbr(resultados,cenarios)
Esta função realiza o calculo do CBR considerando um conjunto de cenários simulados.
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
     <sheet name="Configs" sheetId="1" r:id="rId2"/>
     <sheet name="Dados_Projetados" sheetId="2" r:id="rId3"/>
     <sheet name="Cenarios" sheetId="9" r:id="rId4"/>
-    <sheet name="Parametros" sheetId="4" r:id="rId5"/>
-    <sheet name="Distribuições" sheetId="10" r:id="rId6"/>
-    <sheet name="Custos" sheetId="8" r:id="rId7"/>
-    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId8"/>
+    <sheet name="Parametros_Modular" sheetId="11" r:id="rId5"/>
+    <sheet name="Parametros" sheetId="4" r:id="rId6"/>
+    <sheet name="Distribuições" sheetId="10" r:id="rId7"/>
+    <sheet name="Custos" sheetId="8" r:id="rId8"/>
+    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$H$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Parametros!$A$1:$H$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros_Modular!$A$1:$H$33</definedName>
     <definedName name="Ano_Inicial">Configs!$D$2:$D$2</definedName>
     <definedName name="Anos_a_Serem_Simulados">Configs!$A$2</definedName>
     <definedName name="CategoriaSAT">Configs!$C$2:$C$2</definedName>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="89">
   <si>
     <t>Ano</t>
   </si>
@@ -288,6 +290,18 @@
   </si>
   <si>
     <t>moda (valor mais provável)</t>
+  </si>
+  <si>
+    <t>Tem Crise?</t>
+  </si>
+  <si>
+    <t>Fator Multiplicador</t>
+  </si>
+  <si>
+    <t>Impacto</t>
+  </si>
+  <si>
+    <t>Positivo?</t>
   </si>
 </sst>
 </file>
@@ -789,7 +803,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +896,7 @@
         <v>123412321</v>
       </c>
       <c r="F2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -1383,10 +1397,572 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L33"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2">
+        <f>Parametros!C2*J2</f>
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f>1+K2*L2</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3">
+        <f>Parametros!C3*J3</f>
+        <v>22</v>
+      </c>
+      <c r="D3" s="10">
+        <f>D2*1.1</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J5" si="0">1+K3*L3</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K3" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4">
+        <f>Parametros!C4*J4</f>
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="D4">
+        <v>1E-3</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5">
+        <f>Parametros!C5*J5</f>
+        <v>0.1</v>
+      </c>
+      <c r="D5">
+        <v>1E-3</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="10">
+        <v>20</v>
+      </c>
+      <c r="D7" s="10">
+        <f>D6*1.1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>1E-3</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9">
+        <v>0.05</v>
+      </c>
+      <c r="D9">
+        <v>1E-3</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="10">
+        <v>8</v>
+      </c>
+      <c r="D11" s="10">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12">
+        <v>0.05</v>
+      </c>
+      <c r="D12">
+        <v>0.08</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E17" si="1">D12*1.2</f>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13">
+        <v>0.05</v>
+      </c>
+      <c r="D13">
+        <v>0.08</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>8.4</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="10">
+        <v>9</v>
+      </c>
+      <c r="D15" s="10">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16">
+        <v>0.05</v>
+      </c>
+      <c r="D16">
+        <v>0.08</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17">
+        <v>0.05</v>
+      </c>
+      <c r="D17">
+        <v>0.08</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="33" hidden="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <autoFilter ref="A1:H33">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="SemIniciativa"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,7 +2374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1872,12 +2448,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,7 +2489,7 @@
         <v>2017</v>
       </c>
       <c r="D2" s="4">
-        <v>50000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,7 +2503,7 @@
         <v>2018</v>
       </c>
       <c r="D3" s="4">
-        <v>50000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1941,7 +2517,7 @@
         <v>2019</v>
       </c>
       <c r="D4" s="4">
-        <v>50000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1955,7 +2531,7 @@
         <v>2020</v>
       </c>
       <c r="D5" s="4">
-        <v>50000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1969,7 +2545,7 @@
         <v>2021</v>
       </c>
       <c r="D6" s="4">
-        <v>50000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1984,7 +2560,7 @@
       </c>
       <c r="D7" s="4">
         <f>D2*2</f>
-        <v>100000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1999,7 +2575,7 @@
       </c>
       <c r="D8" s="4">
         <f t="shared" ref="D8:D11" si="0">D3*2</f>
-        <v>100000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2014,7 +2590,7 @@
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2029,7 +2605,7 @@
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2044,7 +2620,7 @@
       </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2058,7 +2634,7 @@
         <v>2017</v>
       </c>
       <c r="D12" s="4">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2072,7 +2648,7 @@
         <v>2018</v>
       </c>
       <c r="D13" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2086,7 +2662,7 @@
         <v>2019</v>
       </c>
       <c r="D14" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2100,7 +2676,7 @@
         <v>2020</v>
       </c>
       <c r="D15" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2114,7 +2690,7 @@
         <v>2021</v>
       </c>
       <c r="D16" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2128,7 +2704,7 @@
         <v>2017</v>
       </c>
       <c r="D17" s="4">
-        <v>50</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,7 +2718,7 @@
         <v>2018</v>
       </c>
       <c r="D18" s="4">
-        <v>20</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2156,7 +2732,7 @@
         <v>2019</v>
       </c>
       <c r="D19" s="4">
-        <v>20</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2170,7 +2746,7 @@
         <v>2020</v>
       </c>
       <c r="D20" s="4">
-        <v>20</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2184,7 +2760,7 @@
         <v>2021</v>
       </c>
       <c r="D21" s="4">
-        <v>20</v>
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
@@ -2192,7 +2768,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
#2 Ajustes para o Calculo do CBR
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -703,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +926,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Layout atualizado separando tabela de resultados dos graficos.
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
     <sheet name="Configs" sheetId="1" r:id="rId2"/>
     <sheet name="Dados_Projetados" sheetId="2" r:id="rId3"/>
     <sheet name="Cenarios" sheetId="9" r:id="rId4"/>
-    <sheet name="Parametros_Modular" sheetId="11" r:id="rId5"/>
-    <sheet name="Parametros" sheetId="4" r:id="rId6"/>
-    <sheet name="Distribuições" sheetId="10" r:id="rId7"/>
-    <sheet name="Custos" sheetId="8" r:id="rId8"/>
-    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId9"/>
+    <sheet name="Parametros" sheetId="4" r:id="rId5"/>
+    <sheet name="Distribuições" sheetId="10" r:id="rId6"/>
+    <sheet name="Custos" sheetId="8" r:id="rId7"/>
+    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Parametros!$A$1:$H$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros_Modular!$A$1:$H$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$H$33</definedName>
     <definedName name="Ano_Inicial">Configs!$D$2:$D$2</definedName>
     <definedName name="Anos_a_Serem_Simulados">Configs!$A$2</definedName>
     <definedName name="CategoriaSAT">Configs!$C$2:$C$2</definedName>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="85">
   <si>
     <t>Ano</t>
   </si>
@@ -290,18 +288,6 @@
   </si>
   <si>
     <t>moda (valor mais provável)</t>
-  </si>
-  <si>
-    <t>Tem Crise?</t>
-  </si>
-  <si>
-    <t>Fator Multiplicador</t>
-  </si>
-  <si>
-    <t>Impacto</t>
-  </si>
-  <si>
-    <t>Positivo?</t>
   </si>
 </sst>
 </file>
@@ -703,7 +689,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -802,9 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -926,7 +912,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,573 +1383,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:L33"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2">
-        <f>Parametros!C2*J2</f>
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <f>1+K2*L2</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K2" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3">
-        <f>Parametros!C3*J3</f>
-        <v>22</v>
-      </c>
-      <c r="D3" s="10">
-        <f>D2*1.1</f>
-        <v>3.3000000000000003</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J5" si="0">1+K3*L3</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K3" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4">
-        <f>Parametros!C4*J4</f>
-        <v>0.11000000000000001</v>
-      </c>
-      <c r="D4">
-        <v>1E-3</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K4" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5">
-        <f>Parametros!C5*J5</f>
-        <v>0.1</v>
-      </c>
-      <c r="D5">
-        <v>1E-3</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K5" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="10">
-        <v>20</v>
-      </c>
-      <c r="D7" s="10">
-        <f>D6*1.1</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8">
-        <v>0.05</v>
-      </c>
-      <c r="D8">
-        <v>1E-3</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9">
-        <v>0.05</v>
-      </c>
-      <c r="D9">
-        <v>1E-3</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="10">
-        <v>8</v>
-      </c>
-      <c r="D11" s="10">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12">
-        <v>0.05</v>
-      </c>
-      <c r="D12">
-        <v>0.08</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ref="E12:E17" si="1">D12*1.2</f>
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13">
-        <v>0.05</v>
-      </c>
-      <c r="D13">
-        <v>0.08</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>7</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>8.4</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="10">
-        <v>9</v>
-      </c>
-      <c r="D15" s="10">
-        <v>10</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I15" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16">
-        <v>0.05</v>
-      </c>
-      <c r="D16">
-        <v>0.08</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17">
-        <v>0.05</v>
-      </c>
-      <c r="D17">
-        <v>0.08</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="33" hidden="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <autoFilter ref="A1:H33">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="SemIniciativa"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2374,7 +1796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2448,17 +1870,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="13" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="4" bestFit="1" customWidth="1"/>
@@ -2489,7 +1911,7 @@
         <v>2017</v>
       </c>
       <c r="D2" s="4">
-        <v>500</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2503,7 +1925,7 @@
         <v>2018</v>
       </c>
       <c r="D3" s="4">
-        <v>500</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2517,7 +1939,7 @@
         <v>2019</v>
       </c>
       <c r="D4" s="4">
-        <v>500</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2531,7 +1953,7 @@
         <v>2020</v>
       </c>
       <c r="D5" s="4">
-        <v>500</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2545,7 +1967,7 @@
         <v>2021</v>
       </c>
       <c r="D6" s="4">
-        <v>500</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2559,8 +1981,7 @@
         <v>2017</v>
       </c>
       <c r="D7" s="4">
-        <f>D2*2</f>
-        <v>1000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2574,8 +1995,7 @@
         <v>2018</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" ref="D8:D11" si="0">D3*2</f>
-        <v>1000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2589,8 +2009,7 @@
         <v>2019</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2604,8 +2023,7 @@
         <v>2020</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2619,8 +2037,7 @@
         <v>2021</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2704,7 +2121,7 @@
         <v>2017</v>
       </c>
       <c r="D17" s="4">
-        <v>1500</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2718,7 +2135,7 @@
         <v>2018</v>
       </c>
       <c r="D18" s="4">
-        <v>1500</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2732,7 +2149,7 @@
         <v>2019</v>
       </c>
       <c r="D19" s="4">
-        <v>1500</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2746,7 +2163,7 @@
         <v>2020</v>
       </c>
       <c r="D20" s="4">
-        <v>1500</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2760,7 +2177,7 @@
         <v>2021</v>
       </c>
       <c r="D21" s="4">
-        <v>1500</v>
+        <v>150000</v>
       </c>
     </row>
   </sheetData>
@@ -2768,7 +2185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Corrigindo dependências de carregar_inputs()
Corrigindo dependências relacionadas aà lista oshcba_options.
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Funções calcular_funcao, calcular_funcoes, chamar_calculo_das_funcoes
Primeira versão das funções calcular_funcao, calcular_funcoes, chamar_calculo_das_funcoes
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="Dados_Projetados" sheetId="2" r:id="rId3"/>
     <sheet name="Cenarios" sheetId="9" r:id="rId4"/>
     <sheet name="Parametros" sheetId="4" r:id="rId5"/>
-    <sheet name="Distribuições" sheetId="10" r:id="rId6"/>
-    <sheet name="Custos" sheetId="8" r:id="rId7"/>
-    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId8"/>
+    <sheet name="Funcoes_Inputs" sheetId="11" r:id="rId6"/>
+    <sheet name="Funcoes_Outputs" sheetId="12" r:id="rId7"/>
+    <sheet name="Distribuições" sheetId="10" r:id="rId8"/>
+    <sheet name="Custos" sheetId="8" r:id="rId9"/>
+    <sheet name="Benefícios_Capturados" sheetId="3" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$H$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$H$22</definedName>
     <definedName name="Ano_Inicial">Configs!$D$2:$D$2</definedName>
     <definedName name="Anos_a_Serem_Simulados">Configs!$A$2</definedName>
     <definedName name="CategoriaSAT">Configs!$C$2:$C$2</definedName>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="98">
   <si>
     <t>Ano</t>
   </si>
@@ -300,6 +302,33 @@
   </si>
   <si>
     <t>Pev_NRelac</t>
+  </si>
+  <si>
+    <t>Funcao</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>calcular_eventos</t>
+  </si>
+  <si>
+    <t>Param_Externo</t>
+  </si>
+  <si>
+    <t>Nev_Tipico</t>
+  </si>
+  <si>
+    <t>Nev_Trajeto</t>
+  </si>
+  <si>
+    <t>Nev_DoenOcup</t>
+  </si>
+  <si>
+    <t>Nev_NRelac</t>
   </si>
 </sst>
 </file>
@@ -362,7 +391,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -381,7 +410,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -806,6 +834,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
@@ -1403,7 +1443,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -1445,185 +1485,185 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <v>10</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <v>3</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14">
-        <v>0</v>
-      </c>
-      <c r="H2" s="14" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13">
+        <v>0</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>20</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <f>D2*1.1</f>
         <v>3.3000000000000003</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14">
-        <v>0</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>0.1</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>1E-3</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14">
-        <v>0</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <v>0.1</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>1E-3</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14">
-        <v>0</v>
-      </c>
-      <c r="H5" s="14" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>10</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>3</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14">
-        <v>0</v>
-      </c>
-      <c r="H6" s="14" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>20</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <f>D6*1.1</f>
         <v>3.3000000000000003</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>0.1</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>1E-3</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <v>0.1</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>1E-3</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14">
-        <v>0</v>
-      </c>
-      <c r="H9" s="14" t="s">
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13">
+        <v>0</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>85</v>
       </c>
       <c r="B10" t="s">
@@ -1635,8 +1675,8 @@
       <c r="D10">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="G10">
         <v>0</v>
       </c>
@@ -1784,18 +1824,165 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H21"/>
+  <autoFilter ref="A1:H22"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1869,7 +2056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -1881,7 +2068,7 @@
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="12" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1892,10 +2079,10 @@
       <c r="B1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1906,7 +2093,7 @@
       <c r="B2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>2017</v>
       </c>
       <c r="D2" s="4">
@@ -1920,7 +2107,7 @@
       <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>2018</v>
       </c>
       <c r="D3" s="4">
@@ -1934,7 +2121,7 @@
       <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="12">
         <v>2019</v>
       </c>
       <c r="D4" s="4">
@@ -1948,7 +2135,7 @@
       <c r="B5" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <v>2020</v>
       </c>
       <c r="D5" s="4">
@@ -1962,7 +2149,7 @@
       <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="12">
         <v>2021</v>
       </c>
       <c r="D6" s="4">
@@ -1976,7 +2163,7 @@
       <c r="B7" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <v>2017</v>
       </c>
       <c r="D7" s="4">
@@ -1990,7 +2177,7 @@
       <c r="B8" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>2018</v>
       </c>
       <c r="D8" s="4">
@@ -2004,7 +2191,7 @@
       <c r="B9" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <v>2019</v>
       </c>
       <c r="D9" s="4">
@@ -2018,7 +2205,7 @@
       <c r="B10" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>2020</v>
       </c>
       <c r="D10" s="4">
@@ -2032,7 +2219,7 @@
       <c r="B11" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="12">
         <v>2021</v>
       </c>
       <c r="D11" s="4">
@@ -2046,7 +2233,7 @@
       <c r="B12" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="12">
         <v>2017</v>
       </c>
       <c r="D12" s="4">
@@ -2060,7 +2247,7 @@
       <c r="B13" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="12">
         <v>2018</v>
       </c>
       <c r="D13" s="4">
@@ -2074,7 +2261,7 @@
       <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <v>2019</v>
       </c>
       <c r="D14" s="4">
@@ -2088,7 +2275,7 @@
       <c r="B15" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="12">
         <v>2020</v>
       </c>
       <c r="D15" s="4">
@@ -2102,7 +2289,7 @@
       <c r="B16" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="12">
         <v>2021</v>
       </c>
       <c r="D16" s="4">
@@ -2116,7 +2303,7 @@
       <c r="B17" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="12">
         <v>2017</v>
       </c>
       <c r="D17" s="4">
@@ -2130,7 +2317,7 @@
       <c r="B18" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="12">
         <v>2018</v>
       </c>
       <c r="D18" s="4">
@@ -2144,7 +2331,7 @@
       <c r="B19" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="12">
         <v>2019</v>
       </c>
       <c r="D19" s="4">
@@ -2158,7 +2345,7 @@
       <c r="B20" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="12">
         <v>2020</v>
       </c>
       <c r="D20" s="4">
@@ -2172,7 +2359,7 @@
       <c r="B21" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="12">
         <v>2021</v>
       </c>
       <c r="D21" s="4">
@@ -2182,16 +2369,4 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Removendo as dependências incorretas
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -307,12 +307,6 @@
     <t>Funcao</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>calcular_eventos</t>
   </si>
   <si>
@@ -329,6 +323,12 @@
   </si>
   <si>
     <t>Nev_NRelac</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Outputs</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1445,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1835,13 +1837,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1851,15 +1853,15 @@
         <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>85</v>
@@ -1871,7 +1873,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
         <v>86</v>
@@ -1883,7 +1885,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
         <v>87</v>
@@ -1895,7 +1897,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
         <v>88</v>
@@ -1907,7 +1909,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1927,7 +1929,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,39 +1944,39 @@
         <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>